<commit_message>
Agregar datos para psicologos en el proyecto
</commit_message>
<xml_diff>
--- a/datos_psicologos_pacientes.xlsx
+++ b/datos_psicologos_pacientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgimenez\PycharmProjects\dashboard_coach_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{39BA8FEC-FA94-4159-A04C-C55DBCF5A719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3ABA02-9C33-4736-9555-EE1364DDB7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{083C8F64-3A61-4DAC-BD07-386E7847610A}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Paciente</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Salir sola una vez en la semana</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>Estar conmigo</t>
   </si>
 </sst>
 </file>
@@ -939,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9179D1-0238-4117-B6AD-092A887AE401}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,6 +1121,26 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45796</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>